<commit_message>
began testing of Rates and Budget
</commit_message>
<xml_diff>
--- a/templates/rate_sheet_template.xlsx
+++ b/templates/rate_sheet_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/code/cost_control/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5AF01777-8D2F-3E44-AEFC-68E5F6FEE18F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D417109C-3989-BD4A-AF40-75E221162D3B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3080" yWindow="2520" windowWidth="27640" windowHeight="16940" xr2:uid="{6DE067EA-3563-2647-BD3B-E49AEA0BEF2F}"/>
   </bookViews>
@@ -60,13 +60,13 @@
     <t>Frank Hardy</t>
   </si>
   <si>
-    <t>&lt;----- date changes on this sheet will go into effect</t>
-  </si>
-  <si>
     <t>Personnel and Labor Rates</t>
   </si>
   <si>
     <t>Owens Lake Dust Mitigation Project</t>
+  </si>
+  <si>
+    <t>&lt;----- date changes on this sheet will go into effect (must be in mm/dd/yy format)</t>
   </si>
 </sst>
 </file>
@@ -678,7 +678,7 @@
   <dimension ref="A2:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -691,12 +691,12 @@
   <sheetData>
     <row r="2" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="B3" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -709,7 +709,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>

</xml_diff>